<commit_message>
re organized the calendar cache to not use static member variables as it made no sense to have the unordered map as static memeber variable
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BBABF5-5A57-4562-A213-B205FC611FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815C0BD-9692-4B10-A099-4332A3ECD4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
@@ -16,6 +16,12 @@
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
     <sheet name="day_count" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="dayCountResult">day_count!$C$54</definedName>
+    <definedName name="vbaDayCount">day_count!$A$52</definedName>
+    <definedName name="vbaEndDate">day_count!$B$54</definedName>
+    <definedName name="vbaStartDate">day_count!$A$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>NYB</t>
   </si>
@@ -911,10 +917,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFECD9EC-9790-480B-9B33-A26F15505398}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:M50"/>
+  <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,6 +2232,33 @@
         <v>180</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>39097</v>
+      </c>
+      <c r="B54" s="1">
+        <v>39112</v>
+      </c>
+      <c r="C54">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
did some minor code cleaning
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815C0BD-9692-4B10-A099-4332A3ECD4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766F104F-A474-4909-A80A-20D403EB5599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,6 @@
     <t>BoxingDay</t>
   </si>
   <si>
-    <t xml:space="preserve">Day After Bosing Day </t>
-  </si>
-  <si>
     <t>nyb</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">Memorial Day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day After Bxsing Day </t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="E5:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,10 +656,10 @@
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="5:12" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L7" t="s">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
         <v>4</v>
@@ -814,10 +814,10 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="5:12" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
@@ -870,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L17" t="s">
         <v>6</v>
@@ -919,8 +919,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,34 +936,34 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="G2" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1718,34 +1718,34 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
       <c r="G27" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="G28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="I28" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2234,18 +2234,18 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
         <v>18</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Saving initial saved work
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766F104F-A474-4909-A80A-20D403EB5599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9ACD25-A43E-4EC4-B314-6C54AC6897FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
     <sheet name="day_count" sheetId="2" r:id="rId2"/>
+    <sheet name="ComputeDate" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="dayCountResult">day_count!$C$54</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>NYB</t>
   </si>
@@ -110,6 +111,27 @@
   </si>
   <si>
     <t xml:space="preserve">Day After Bxsing Day </t>
+  </si>
+  <si>
+    <t>Base_Date</t>
+  </si>
+  <si>
+    <t>Tenor</t>
+  </si>
+  <si>
+    <t>Adjustment_Rule</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>4M</t>
   </si>
 </sst>
 </file>
@@ -623,8 +645,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="E5:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,8 +941,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,4 +2284,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C45751-0031-44E3-951D-7C59C3883439}">
+  <dimension ref="B2:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
+        <v>Dictionary_ComputeDate_$1$2:4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <f>_xll.oxlComputeDate(B3:C6)</f>
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <f>_xll.oxlComputeDate(B3:B6,C3:C6)</f>
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <f>_xll.oxlComputeDate(C2)</f>
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="str">
+        <f>_xll.oxlComputeDate(C3,C4,C5,C6)</f>
+        <v>ERROR:Not an Excel String Type line check the input: xloper_converter.cpp line 244 LPXloperToStr()</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished dictionary initial autogen
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAEAE15-7062-4804-81B9-F148CEEFE4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1123973F-FFCD-487A-9E3A-1E8D8E092D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
@@ -128,10 +128,10 @@
     <t/>
   </si>
   <si>
-    <t>MF</t>
-  </si>
-  <si>
-    <t>6M</t>
+    <t>8M</t>
+  </si>
+  <si>
+    <t>Following</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>ComputeDate!C2</f>
-        <v>Dictionary_ComputeDate_$1$2:2</v>
+        <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -947,8 +947,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2296,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C45751-0031-44E3-951D-7C59C3883439}">
   <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,12 +2305,13 @@
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C2" t="str">
         <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
-        <v>Dictionary_ComputeDate_$1$2:2</v>
+        <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -2325,7 +2326,7 @@
         <v>Adjustment_Rule</v>
       </c>
       <c r="G3" t="str">
-        <v>MF</v>
+        <v>Following</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -2333,12 +2334,12 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="str">
         <v>Base_Date</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>45163</v>
       </c>
     </row>
@@ -2347,7 +2348,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" t="str">
         <v>Calendar</v>
@@ -2367,7 +2368,7 @@
         <v>Tenor</v>
       </c>
       <c r="G6" t="str">
-        <v>6M</v>
+        <v>8M</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -2378,25 +2379,25 @@
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <f>_xll.oxlComputeDate(B3:C6)</f>
-        <v>45348</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <f>_xll.oxlComputeDate(B3:B6,C3:C6)</f>
-        <v>45348</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <f>_xll.oxlComputeDate(C2)</f>
-        <v>45348</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <f>_xll.oxlComputeDate(C3,C4,C5,C6)</f>
-        <v>45348</v>
+        <v>45407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished inital upgrade to msvs 2026 but having issues with the include gtest gtest.h
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1123973F-FFCD-487A-9E3A-1E8D8E092D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690E2B6E-40B2-4123-956F-CD0ECBE5D4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
@@ -649,25 +649,25 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
         <f>ComputeDate!C2</f>
         <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -690,7 +690,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F6" s="1">
         <v>44746</v>
       </c>
@@ -713,7 +713,7 @@
         <v>45074</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>0</v>
       </c>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>1</v>
       </c>
@@ -792,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>4</v>
       </c>
@@ -848,7 +848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>6</v>
       </c>
@@ -904,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
@@ -947,34 +947,34 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -984,17 +984,17 @@
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>39097</v>
       </c>
@@ -1017,20 +1017,20 @@
         <f>D4-E4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>39097</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>39112</v>
       </c>
-      <c r="I4" s="3">
-        <f>_xll.oxlComputeDayCount(G4,H4,G$2)</f>
+      <c r="J4" s="3">
+        <f>_xll.oxlComputeDayCount(H4,I4,H$2)</f>
         <v>15</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>39097</v>
       </c>
@@ -1053,18 +1053,18 @@
         <f t="shared" ref="F5:F25" si="0">D5-E5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>39097</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>39128</v>
       </c>
-      <c r="I5" s="3">
-        <f>_xll.oxlComputeDayCount(G5,H5,G$2)</f>
+      <c r="J5" s="3">
+        <f>_xll.oxlComputeDayCount(H5,I5,H$2)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>39097</v>
       </c>
@@ -1087,18 +1087,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>39097</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>39278</v>
       </c>
-      <c r="I6" s="3">
-        <f>_xll.oxlComputeDayCount(G6,H6,G$2)</f>
+      <c r="J6" s="3">
+        <f>_xll.oxlComputeDayCount(H6,I6,H$2)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>39355</v>
       </c>
@@ -1121,18 +1121,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>39355</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>39538</v>
       </c>
-      <c r="I7" s="3">
-        <f>_xll.oxlComputeDayCount(G7,H7,G$2)</f>
+      <c r="J7" s="3">
+        <f>_xll.oxlComputeDayCount(H7,I7,H$2)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>39355</v>
       </c>
@@ -1155,18 +1155,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>39355</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>39386</v>
       </c>
-      <c r="I8" s="3">
-        <f>_xll.oxlComputeDayCount(G8,H8,G$2)</f>
+      <c r="J8" s="3">
+        <f>_xll.oxlComputeDayCount(H8,I8,H$2)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>39355</v>
       </c>
@@ -1189,18 +1189,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>39355</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>39721</v>
       </c>
-      <c r="I9" s="3">
-        <f>_xll.oxlComputeDayCount(G9,H9,G$2)</f>
+      <c r="J9" s="3">
+        <f>_xll.oxlComputeDayCount(H9,I9,H$2)</f>
         <v>360</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>39097</v>
       </c>
@@ -1223,18 +1223,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>39097</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>39113</v>
       </c>
-      <c r="I10" s="3">
-        <f>_xll.oxlComputeDayCount(G10,H10,G$2)</f>
+      <c r="J10" s="3">
+        <f>_xll.oxlComputeDayCount(H10,I10,H$2)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>39113</v>
       </c>
@@ -1257,18 +1257,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>39113</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>39141</v>
       </c>
-      <c r="I11" s="3">
-        <f>_xll.oxlComputeDayCount(G11,H11,G$2)</f>
+      <c r="J11" s="3">
+        <f>_xll.oxlComputeDayCount(H11,I11,H$2)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>39141</v>
       </c>
@@ -1291,18 +1291,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>39141</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>39172</v>
       </c>
-      <c r="I12" s="3">
-        <f>_xll.oxlComputeDayCount(G12,H12,G$2)</f>
+      <c r="J12" s="3">
+        <f>_xll.oxlComputeDayCount(H12,I12,H$2)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>38960</v>
       </c>
@@ -1325,18 +1325,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="4">
         <v>38960</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>39141</v>
       </c>
-      <c r="I13" s="3">
-        <f>_xll.oxlComputeDayCount(G13,H13,G$2)</f>
+      <c r="J13" s="3">
+        <f>_xll.oxlComputeDayCount(H13,I13,H$2)</f>
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>39141</v>
       </c>
@@ -1359,18 +1359,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>39141</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>39325</v>
       </c>
-      <c r="I14" s="3">
-        <f>_xll.oxlComputeDayCount(G14,H14,G$2)</f>
+      <c r="J14" s="3">
+        <f>_xll.oxlComputeDayCount(H14,I14,H$2)</f>
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>39127</v>
       </c>
@@ -1393,18 +1393,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>39127</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>39141</v>
       </c>
-      <c r="I15" s="3">
-        <f>_xll.oxlComputeDayCount(G15,H15,G$2)</f>
+      <c r="J15" s="3">
+        <f>_xll.oxlComputeDayCount(H15,I15,H$2)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>39139</v>
       </c>
@@ -1427,18 +1427,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>39139</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>39507</v>
       </c>
-      <c r="I16" s="3">
-        <f>_xll.oxlComputeDayCount(G16,H16,G$2)</f>
+      <c r="J16" s="3">
+        <f>_xll.oxlComputeDayCount(H16,I16,H$2)</f>
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>39507</v>
       </c>
@@ -1461,18 +1461,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>39507</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>39872</v>
       </c>
-      <c r="I17" s="3">
-        <f>_xll.oxlComputeDayCount(G17,H17,G$2)</f>
+      <c r="J17" s="3">
+        <f>_xll.oxlComputeDayCount(H17,I17,H$2)</f>
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>39507</v>
       </c>
@@ -1495,18 +1495,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>39507</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>39537</v>
       </c>
-      <c r="I18" s="3">
-        <f>_xll.oxlComputeDayCount(G18,H18,G$2)</f>
+      <c r="J18" s="3">
+        <f>_xll.oxlComputeDayCount(H18,I18,H$2)</f>
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>39507</v>
       </c>
@@ -1529,18 +1529,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>39507</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>39538</v>
       </c>
-      <c r="I19" s="3">
-        <f>_xll.oxlComputeDayCount(G19,H19,G$2)</f>
+      <c r="J19" s="3">
+        <f>_xll.oxlComputeDayCount(H19,I19,H$2)</f>
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>39141</v>
       </c>
@@ -1563,18 +1563,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>39141</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>39146</v>
       </c>
-      <c r="I20" s="3">
-        <f>_xll.oxlComputeDayCount(G20,H20,G$2)</f>
+      <c r="J20" s="3">
+        <f>_xll.oxlComputeDayCount(H20,I20,H$2)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>39386</v>
       </c>
@@ -1597,18 +1597,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>39386</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>39414</v>
       </c>
-      <c r="I21" s="3">
-        <f>_xll.oxlComputeDayCount(G21,H21,G$2)</f>
+      <c r="J21" s="3">
+        <f>_xll.oxlComputeDayCount(H21,I21,H$2)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>39325</v>
       </c>
@@ -1631,18 +1631,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="4">
+      <c r="H22" s="4">
         <v>39325</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>39507</v>
       </c>
-      <c r="I22" s="3">
-        <f>_xll.oxlComputeDayCount(G22,H22,G$2)</f>
+      <c r="J22" s="3">
+        <f>_xll.oxlComputeDayCount(H22,I22,H$2)</f>
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>39507</v>
       </c>
@@ -1665,18 +1665,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>39507</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>39691</v>
       </c>
-      <c r="I23" s="3">
-        <f>_xll.oxlComputeDayCount(G23,H23,G$2)</f>
+      <c r="J23" s="3">
+        <f>_xll.oxlComputeDayCount(H23,I23,H$2)</f>
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>39691</v>
       </c>
@@ -1699,18 +1699,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>39691</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>39872</v>
       </c>
-      <c r="I24" s="3">
-        <f>_xll.oxlComputeDayCount(G24,H24,G$2)</f>
+      <c r="J24" s="3">
+        <f>_xll.oxlComputeDayCount(H24,I24,H$2)</f>
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>39872</v>
       </c>
@@ -1733,30 +1733,30 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="5">
+      <c r="H25" s="5">
         <v>39872</v>
       </c>
-      <c r="H25" s="6">
+      <c r="I25" s="6">
         <v>40056</v>
       </c>
-      <c r="I25" s="7">
-        <f>_xll.oxlComputeDayCount(G25,H25,G$2)</f>
+      <c r="J25" s="7">
+        <f>_xll.oxlComputeDayCount(H25,I25,H$2)</f>
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
-      <c r="G27" s="12" t="s">
+      <c r="H27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1766,17 +1766,17 @@
       <c r="C28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="I28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>39097</v>
       </c>
@@ -1787,18 +1787,30 @@
         <f>_xll.oxlComputeDayCount(A29,B29,A$27)</f>
         <v>15</v>
       </c>
-      <c r="G29" s="9">
+      <c r="D29">
+        <f t="shared" ref="D29:D50" si="2">C29/360</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E29">
+        <f>_xll.oxlComputeYearFraction(A29,B29,"act/360")</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F29">
+        <f>E29-D29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
         <v>39097</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I29" s="10">
         <v>39112</v>
       </c>
-      <c r="I29" s="11">
-        <f>_xll.oxlComputeDayCount(G29,H29,G$27)</f>
+      <c r="J29" s="11">
+        <f>_xll.oxlComputeDayCount(H29,I29,H$27)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>39097</v>
       </c>
@@ -1809,18 +1821,30 @@
         <f>_xll.oxlComputeDayCount(A30,B30,A$27)</f>
         <v>31</v>
       </c>
-      <c r="G30" s="4">
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="E30">
+        <f>_xll.oxlComputeYearFraction(A30,B30,"act/360")</f>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:F50" si="3">E30-D30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
         <v>39097</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>39128</v>
       </c>
-      <c r="I30" s="3">
-        <f>_xll.oxlComputeDayCount(G30,H30,G$27)</f>
+      <c r="J30" s="3">
+        <f>_xll.oxlComputeDayCount(H30,I30,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>39097</v>
       </c>
@@ -1831,18 +1855,30 @@
         <f>_xll.oxlComputeDayCount(A31,B31,A$27)</f>
         <v>181</v>
       </c>
-      <c r="G31" s="4">
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="E31">
+        <f>_xll.oxlComputeYearFraction(A31,B31,"act/360")</f>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
         <v>39097</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>39278</v>
       </c>
-      <c r="I31" s="3">
-        <f>_xll.oxlComputeDayCount(G31,H31,G$27)</f>
+      <c r="J31" s="3">
+        <f>_xll.oxlComputeDayCount(H31,I31,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>39355</v>
       </c>
@@ -1853,18 +1889,30 @@
         <f>_xll.oxlComputeDayCount(A32,B32,A$27)</f>
         <v>183</v>
       </c>
-      <c r="G32" s="4">
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="E32">
+        <f>_xll.oxlComputeYearFraction(A32,B32,"act/360")</f>
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
         <v>39355</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>39538</v>
       </c>
-      <c r="I32" s="3">
-        <f>_xll.oxlComputeDayCount(G32,H32,G$27)</f>
+      <c r="J32" s="3">
+        <f>_xll.oxlComputeDayCount(H32,I32,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>39355</v>
       </c>
@@ -1875,18 +1923,30 @@
         <f>_xll.oxlComputeDayCount(A33,B33,A$27)</f>
         <v>31</v>
       </c>
-      <c r="G33" s="4">
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="E33">
+        <f>_xll.oxlComputeYearFraction(A33,B33,"act/360")</f>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
         <v>39355</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>39386</v>
       </c>
-      <c r="I33" s="3">
-        <f>_xll.oxlComputeDayCount(G33,H33,G$27)</f>
+      <c r="J33" s="3">
+        <f>_xll.oxlComputeDayCount(H33,I33,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>39355</v>
       </c>
@@ -1897,18 +1957,30 @@
         <f>_xll.oxlComputeDayCount(A34,B34,A$27)</f>
         <v>366</v>
       </c>
-      <c r="G34" s="4">
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>1.0166666666666666</v>
+      </c>
+      <c r="E34">
+        <f>_xll.oxlComputeYearFraction(A34,B34,"act/360")</f>
+        <v>1.0166666666666666</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
         <v>39355</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>39721</v>
       </c>
-      <c r="I34" s="3">
-        <f>_xll.oxlComputeDayCount(G34,H34,G$27)</f>
+      <c r="J34" s="3">
+        <f>_xll.oxlComputeDayCount(H34,I34,H$27)</f>
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>39097</v>
       </c>
@@ -1919,18 +1991,30 @@
         <f>_xll.oxlComputeDayCount(A35,B35,A$27)</f>
         <v>16</v>
       </c>
-      <c r="G35" s="4">
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="E35">
+        <f>_xll.oxlComputeYearFraction(A35,B35,"act/360")</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="4">
         <v>39097</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>39113</v>
       </c>
-      <c r="I35" s="3">
-        <f>_xll.oxlComputeDayCount(G35,H35,G$27)</f>
+      <c r="J35" s="3">
+        <f>_xll.oxlComputeDayCount(H35,I35,H$27)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>39113</v>
       </c>
@@ -1941,18 +2025,30 @@
         <f>_xll.oxlComputeDayCount(A36,B36,A$27)</f>
         <v>28</v>
       </c>
-      <c r="G36" s="4">
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="E36">
+        <f>_xll.oxlComputeYearFraction(A36,B36,"act/360")</f>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
         <v>39113</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>39141</v>
       </c>
-      <c r="I36" s="3">
-        <f>_xll.oxlComputeDayCount(G36,H36,G$27)</f>
+      <c r="J36" s="3">
+        <f>_xll.oxlComputeDayCount(H36,I36,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>39141</v>
       </c>
@@ -1963,18 +2059,30 @@
         <f>_xll.oxlComputeDayCount(A37,B37,A$27)</f>
         <v>31</v>
       </c>
-      <c r="G37" s="4">
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="E37">
+        <f>_xll.oxlComputeYearFraction(A37,B37,"act/360")</f>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
         <v>39141</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>39172</v>
       </c>
-      <c r="I37" s="3">
-        <f>_xll.oxlComputeDayCount(G37,H37,G$27)</f>
+      <c r="J37" s="3">
+        <f>_xll.oxlComputeDayCount(H37,I37,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>38960</v>
       </c>
@@ -1985,18 +2093,30 @@
         <f>_xll.oxlComputeDayCount(A38,B38,A$27)</f>
         <v>181</v>
       </c>
-      <c r="G38" s="4">
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="E38">
+        <f>_xll.oxlComputeYearFraction(A38,B38,"act/360")</f>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
         <v>38960</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>39141</v>
       </c>
-      <c r="I38" s="3">
-        <f>_xll.oxlComputeDayCount(G38,H38,G$27)</f>
+      <c r="J38" s="3">
+        <f>_xll.oxlComputeDayCount(H38,I38,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>39141</v>
       </c>
@@ -2007,18 +2127,30 @@
         <f>_xll.oxlComputeDayCount(A39,B39,A$27)</f>
         <v>184</v>
       </c>
-      <c r="G39" s="4">
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="E39">
+        <f>_xll.oxlComputeYearFraction(A39,B39,"act/360")</f>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
         <v>39141</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>39325</v>
       </c>
-      <c r="I39" s="3">
-        <f>_xll.oxlComputeDayCount(G39,H39,G$27)</f>
+      <c r="J39" s="3">
+        <f>_xll.oxlComputeDayCount(H39,I39,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39127</v>
       </c>
@@ -2029,18 +2161,30 @@
         <f>_xll.oxlComputeDayCount(A40,B40,A$27)</f>
         <v>14</v>
       </c>
-      <c r="G40" s="4">
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="E40">
+        <f>_xll.oxlComputeYearFraction(A40,B40,"act/360")</f>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
         <v>39127</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>39141</v>
       </c>
-      <c r="I40" s="3">
-        <f>_xll.oxlComputeDayCount(G40,H40,G$27)</f>
+      <c r="J40" s="3">
+        <f>_xll.oxlComputeDayCount(H40,I40,H$27)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39139</v>
       </c>
@@ -2051,18 +2195,30 @@
         <f>_xll.oxlComputeDayCount(A41,B41,A$27)</f>
         <v>368</v>
       </c>
-      <c r="G41" s="4">
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>1.0222222222222221</v>
+      </c>
+      <c r="E41">
+        <f>_xll.oxlComputeYearFraction(A41,B41,"act/360")</f>
+        <v>1.0222222222222221</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
         <v>39139</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>39507</v>
       </c>
-      <c r="I41" s="3">
-        <f>_xll.oxlComputeDayCount(G41,H41,G$27)</f>
+      <c r="J41" s="3">
+        <f>_xll.oxlComputeDayCount(H41,I41,H$27)</f>
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39507</v>
       </c>
@@ -2073,18 +2229,30 @@
         <f>_xll.oxlComputeDayCount(A42,B42,A$27)</f>
         <v>365</v>
       </c>
-      <c r="G42" s="4">
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>1.0138888888888888</v>
+      </c>
+      <c r="E42">
+        <f>_xll.oxlComputeYearFraction(A42,B42,"act/360")</f>
+        <v>1.0138888888888888</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
         <v>39507</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>39872</v>
       </c>
-      <c r="I42" s="3">
-        <f>_xll.oxlComputeDayCount(G42,H42,G$27)</f>
+      <c r="J42" s="3">
+        <f>_xll.oxlComputeDayCount(H42,I42,H$27)</f>
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>39507</v>
       </c>
@@ -2095,18 +2263,30 @@
         <f>_xll.oxlComputeDayCount(A43,B43,A$27)</f>
         <v>30</v>
       </c>
-      <c r="G43" s="4">
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E43">
+        <f>_xll.oxlComputeYearFraction(A43,B43,"act/360")</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
         <v>39507</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>39537</v>
       </c>
-      <c r="I43" s="3">
-        <f>_xll.oxlComputeDayCount(G43,H43,G$27)</f>
+      <c r="J43" s="3">
+        <f>_xll.oxlComputeDayCount(H43,I43,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39507</v>
       </c>
@@ -2117,18 +2297,30 @@
         <f>_xll.oxlComputeDayCount(A44,B44,A$27)</f>
         <v>31</v>
       </c>
-      <c r="G44" s="4">
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="E44">
+        <f>_xll.oxlComputeYearFraction(A44,B44,"act/360")</f>
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="4">
         <v>39507</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>39538</v>
       </c>
-      <c r="I44" s="3">
-        <f>_xll.oxlComputeDayCount(G44,H44,G$27)</f>
+      <c r="J44" s="3">
+        <f>_xll.oxlComputeDayCount(H44,I44,H$27)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>39141</v>
       </c>
@@ -2139,18 +2331,30 @@
         <f>_xll.oxlComputeDayCount(A45,B45,A$27)</f>
         <v>5</v>
       </c>
-      <c r="G45" s="4">
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E45">
+        <f>_xll.oxlComputeYearFraction(A45,B45,"act/360")</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="4">
         <v>39141</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>39146</v>
       </c>
-      <c r="I45" s="3">
-        <f>_xll.oxlComputeDayCount(G45,H45,G$27)</f>
+      <c r="J45" s="3">
+        <f>_xll.oxlComputeDayCount(H45,I45,H$27)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>39386</v>
       </c>
@@ -2161,18 +2365,30 @@
         <f>_xll.oxlComputeDayCount(A46,B46,A$27)</f>
         <v>28</v>
       </c>
-      <c r="G46" s="4">
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="E46">
+        <f>_xll.oxlComputeYearFraction(A46,B46,"act/360")</f>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="4">
         <v>39386</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>39414</v>
       </c>
-      <c r="I46" s="3">
-        <f>_xll.oxlComputeDayCount(G46,H46,G$27)</f>
+      <c r="J46" s="3">
+        <f>_xll.oxlComputeDayCount(H46,I46,H$27)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>39325</v>
       </c>
@@ -2183,18 +2399,30 @@
         <f>_xll.oxlComputeDayCount(A47,B47,A$27)</f>
         <v>182</v>
       </c>
-      <c r="G47" s="4">
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="E47">
+        <f>_xll.oxlComputeYearFraction(A47,B47,"act/360")</f>
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="4">
         <v>39325</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>39507</v>
       </c>
-      <c r="I47" s="3">
-        <f>_xll.oxlComputeDayCount(G47,H47,G$27)</f>
+      <c r="J47" s="3">
+        <f>_xll.oxlComputeDayCount(H47,I47,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39507</v>
       </c>
@@ -2205,18 +2433,30 @@
         <f>_xll.oxlComputeDayCount(A48,B48,A$27)</f>
         <v>184</v>
       </c>
-      <c r="G48" s="4">
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="E48">
+        <f>_xll.oxlComputeYearFraction(A48,B48,"act/360")</f>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
         <v>39507</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <v>39691</v>
       </c>
-      <c r="I48" s="3">
-        <f>_xll.oxlComputeDayCount(G48,H48,G$27)</f>
+      <c r="J48" s="3">
+        <f>_xll.oxlComputeDayCount(H48,I48,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>39691</v>
       </c>
@@ -2227,18 +2467,30 @@
         <f>_xll.oxlComputeDayCount(A49,B49,A$27)</f>
         <v>181</v>
       </c>
-      <c r="G49" s="4">
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="E49">
+        <f>_xll.oxlComputeYearFraction(A49,B49,"act/360")</f>
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="4">
         <v>39691</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>39872</v>
       </c>
-      <c r="I49" s="3">
-        <f>_xll.oxlComputeDayCount(G49,H49,G$27)</f>
+      <c r="J49" s="3">
+        <f>_xll.oxlComputeDayCount(H49,I49,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>39872</v>
       </c>
@@ -2249,23 +2501,35 @@
         <f>_xll.oxlComputeDayCount(A50,B50,A$27)</f>
         <v>184</v>
       </c>
-      <c r="G50" s="5">
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="E50">
+        <f>_xll.oxlComputeYearFraction(A50,B50,"act/360")</f>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
         <v>39872</v>
       </c>
-      <c r="H50" s="6">
+      <c r="I50" s="6">
         <v>40056</v>
       </c>
-      <c r="I50" s="7">
-        <f>_xll.oxlComputeDayCount(G50,H50,G$27)</f>
+      <c r="J50" s="7">
+        <f>_xll.oxlComputeDayCount(H50,I50,H$27)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>39097</v>
       </c>
@@ -2300,21 +2564,21 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
         <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
         <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -2329,7 +2593,7 @@
         <v>Following</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -2343,7 +2607,7 @@
         <v>45163</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -2357,7 +2621,7 @@
         <v>NYB</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -2371,30 +2635,30 @@
         <v>8M</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f>_xll.oxlComputeDate(B3:C6)</f>
         <v>45407</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f>_xll.oxlComputeDate(B3:B6,C3:C6)</f>
         <v>45407</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f>_xll.oxlComputeDate(C2)</f>
         <v>45407</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f>_xll.oxlComputeDate(C3,C4,C5,C6)</f>
         <v>45407</v>

</xml_diff>

<commit_message>
finshed intial draft for business date formula
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ExcelPy\OdinAnalytics\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1123973F-FFCD-487A-9E3A-1E8D8E092D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6AE0C-D2CC-411A-B77D-CB75AF6167DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>NYB</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Following</t>
+  </si>
+  <si>
+    <t>NumDays</t>
   </si>
 </sst>
 </file>
@@ -649,25 +652,25 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
         <f>ComputeDate!C2</f>
         <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -690,7 +693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F6" s="1">
         <v>44746</v>
       </c>
@@ -713,7 +716,7 @@
         <v>45074</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>0</v>
       </c>
@@ -736,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
@@ -769,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>1</v>
       </c>
@@ -792,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
@@ -825,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>4</v>
       </c>
@@ -848,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
@@ -881,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>6</v>
       </c>
@@ -904,7 +907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
@@ -947,22 +950,22 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -974,7 +977,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -994,7 +997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>39097</v>
       </c>
@@ -1030,7 +1033,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>39097</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>39097</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>39355</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>39355</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>39355</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>39097</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>39113</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>39141</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>38960</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>39141</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>39127</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>39139</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>39507</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>39507</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>39507</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>39141</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>39386</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>39325</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>39507</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>39691</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>39872</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>20</v>
       </c>
@@ -1756,7 +1759,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>39097</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>39097</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>39097</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>39355</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>39355</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>39355</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>39097</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>39113</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>39141</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>38960</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>39141</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39127</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39139</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39507</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>39507</v>
       </c>
@@ -2106,7 +2109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39507</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>39141</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>39386</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>39325</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39507</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>39691</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>39872</v>
       </c>
@@ -2260,12 +2263,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>39097</v>
       </c>
@@ -2294,110 +2297,193 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C45751-0031-44E3-951D-7C59C3883439}">
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
         <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
         <v>Dictionary_ComputeDate_$1$2:9</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K2" t="str">
+        <f>_xll.oxlDictionary(J3:J5,K3:K5)</f>
+        <v>Dictionary_ComputeDate_$1$10:4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="1">
         <v>45163</v>
       </c>
+      <c r="E3" t="str">
+        <f t="array" ref="E3:F6">_xll.oxlDisplay(C2)</f>
+        <v>Adjustment_Rule</v>
+      </c>
       <c r="F3" t="str">
-        <f t="array" ref="F3:G6">_xll.oxlDisplay(C2)</f>
-        <v>Adjustment_Rule</v>
-      </c>
-      <c r="G3" t="str">
         <v>Following</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1">
+        <v>46336</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="str">
+      <c r="E4" t="str">
         <v>Base_Date</v>
       </c>
-      <c r="G4" s="1">
+      <c r="F4" s="1">
         <v>45163</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
+      <c r="E5" t="str">
+        <v>Calendar</v>
+      </c>
       <c r="F5" t="str">
-        <v>Calendar</v>
-      </c>
-      <c r="G5" t="str">
         <v>NYB</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
+      <c r="E6" t="str">
+        <v>Tenor</v>
+      </c>
       <c r="F6" t="str">
-        <v>Tenor</v>
-      </c>
-      <c r="G6" t="str">
         <v>8M</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f>_xll.oxlComputeDate(B3:C6)</f>
         <v>45407</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <f>_xll.oxlAddBusinessDays(K3,K4,K5)</f>
+        <v>46344</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f>_xll.oxlComputeDate(B3:B6,C3:C6)</f>
         <v>45407</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <f>_xll.oxlAddBusinessDays(J3:J5,K3:K5)</f>
+        <v>46344</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f>_xll.oxlComputeDate(C2)</f>
         <v>45407</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <f>_xll.oxlAddBusinessDays(K2)</f>
+        <v>46344</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f>_xll.oxlComputeDate(C3,C4,C5,C6)</f>
         <v>45407</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f>_xll.oxlDictionary(J13:J15,K13:K15)</f>
+        <v>Dictionary_ComputeDate_$11$10:1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="1">
+        <v>46344</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="1">
+        <f>_xll.oxlAddBusinessDays(K13,K14,K15)</f>
+        <v>46336</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="1">
+        <f>_xll.oxlAddBusinessDays(J13:J15,K13:K15)</f>
+        <v>46336</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="1">
+        <f>_xll.oxlAddBusinessDays(K12)</f>
+        <v>46336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished overlaoding operator for business_date_formula with unit test. Also made changes tot he .xlam to look at one file level higher for the dll's. saving current work
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6AE0C-D2CC-411A-B77D-CB75AF6167DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B342B-711F-4773-91C8-8725737A1C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>Following</t>
   </si>
   <si>
-    <t>NumDays</t>
+    <t>Days</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
         <f>ComputeDate!C2</f>
-        <v>Dictionary_ComputeDate_$1$2:9</v>
+        <v>Dictionary_ComputeDate_$1$2:0</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,11 +2315,11 @@
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
         <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
-        <v>Dictionary_ComputeDate_$1$2:9</v>
+        <v>Dictionary_ComputeDate_$1$2:0</v>
       </c>
       <c r="K2" t="str">
         <f>_xll.oxlDictionary(J3:J5,K3:K5)</f>
-        <v>Dictionary_ComputeDate_$1$10:4</v>
+        <v>Dictionary_ComputeDate_$1$10:0</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K12" t="str">
         <f>_xll.oxlDictionary(J13:J15,K13:K15)</f>
-        <v>Dictionary_ComputeDate_$11$10:1</v>
+        <v>Dictionary_ComputeDate_$11$10:0</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished updating the inline declaration and cleaning up unit test
</commit_message>
<xml_diff>
--- a/sheets/time_test_sheet.xlsx
+++ b/sheets/time_test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OdinAnalytics\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B342B-711F-4773-91C8-8725737A1C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3590F24-EC0D-4CCC-8F30-427014F9C3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4F0FB8F6-FBCA-4404-B166-FFC6556ED016}"/>
   </bookViews>
   <sheets>
     <sheet name="boolean_logic_dates" sheetId="1" r:id="rId1"/>
@@ -652,25 +652,25 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>ComputeDate!C2</f>
         <v>Dictionary_ComputeDate_$1$2:0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -693,7 +693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F6" s="1">
         <v>44746</v>
       </c>
@@ -716,7 +716,7 @@
         <v>45074</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>0</v>
       </c>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>1</v>
       </c>
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>4</v>
       </c>
@@ -851,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>6</v>
       </c>
@@ -907,7 +907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
@@ -954,18 +954,18 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -997,7 +997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>39097</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>39097</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>39097</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>39355</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>39355</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>39355</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>39097</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>39113</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>39141</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>38960</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>39141</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>39127</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>39139</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>39507</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>39507</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>39507</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>39141</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>39386</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>39325</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>39507</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>39691</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>39872</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>20</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>39097</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>39097</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>39097</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>39355</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>39355</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>39355</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>39097</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>39113</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>39141</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>38960</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>39141</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39127</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39139</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>39507</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>39507</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>39507</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>39141</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>39386</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>39325</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>39507</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>39691</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>39872</v>
       </c>
@@ -2263,12 +2263,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>39097</v>
       </c>
@@ -2300,29 +2300,29 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C2" t="str">
         <f>_xll.oxlDictionary(B3:B6,C3:C6)</f>
         <v>Dictionary_ComputeDate_$1$2:0</v>
       </c>
       <c r="K2" t="str">
         <f>_xll.oxlDictionary(J3:J5,K3:K5)</f>
-        <v>Dictionary_ComputeDate_$1$10:0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+        <v>Dictionary_ComputeDate_$1$10:1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>46336</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -2397,12 +2397,12 @@
         <v>8M</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <f>_xll.oxlComputeDate(B3:C6)</f>
         <v>45407</v>
@@ -2412,7 +2412,7 @@
         <v>46344</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <f>_xll.oxlComputeDate(B3:B6,C3:C6)</f>
         <v>45407</v>
@@ -2422,7 +2422,7 @@
         <v>46344</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <f>_xll.oxlComputeDate(C2)</f>
         <v>45407</v>
@@ -2432,19 +2432,19 @@
         <v>46344</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <f>_xll.oxlComputeDate(C3,C4,C5,C6)</f>
         <v>45407</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K12" t="str">
         <f>_xll.oxlDictionary(J13:J15,K13:K15)</f>
         <v>Dictionary_ComputeDate_$11$10:0</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
         <v>26</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>46344</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
         <v>33</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
         <v>29</v>
       </c>
@@ -2468,19 +2468,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="1">
         <f>_xll.oxlAddBusinessDays(K13,K14,K15)</f>
         <v>46336</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="1">
         <f>_xll.oxlAddBusinessDays(J13:J15,K13:K15)</f>
         <v>46336</v>
       </c>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" s="1">
         <f>_xll.oxlAddBusinessDays(K12)</f>
         <v>46336</v>

</xml_diff>